<commit_message>
bugfix in Časové údaje, to allow more than 3 places
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\PycharmProjects\CarsFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB454AA3-E8D0-48FE-B962-3A953B8AE033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B11ABEF-DE20-4FC1-9E62-3DE75EA53C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{F5FDD420-4A2D-4EC0-801E-60E8B6A79417}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>15.10.</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>úprava histogramu</t>
+  </si>
+  <si>
+    <t>bugfix in Časové údaje</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="B2:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +797,15 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="4">
+        <v>45415</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
@@ -802,7 +813,7 @@
       </c>
       <c r="E36" s="3">
         <f>SUM(E30:E35)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -819,7 +830,7 @@
       </c>
       <c r="E38" s="3">
         <f>E36*300</f>
-        <v>2700</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated timesheet.xlsx - invoice sent
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\PycharmProjects\CarsFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B11ABEF-DE20-4FC1-9E62-3DE75EA53C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF69ADE4-C1E6-4DAE-92FE-B0F8348175EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{F5FDD420-4A2D-4EC0-801E-60E8B6A79417}"/>
   </bookViews>
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B7312E-7458-4F53-AAD2-0B844DD46A77}">
-  <dimension ref="B2:F38"/>
+  <dimension ref="B2:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,29 +807,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3">
+        <f>SUM(E30:E34)</f>
+        <v>10</v>
+      </c>
+    </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="3">
-        <f>SUM(E30:E35)</f>
-        <v>10</v>
+      <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36">
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="3">
-        <f>E36*300</f>
+      <c r="E37" s="3">
+        <f>E35*300</f>
         <v>3000</v>
       </c>
     </row>

</xml_diff>